<commit_message>
Portfolio: Added Next and Previous functionality
* relying on auto generated sort orders, as the spreadsheet can skip items.
* detect previous and net items shows and hides pervious and next buttons.
</commit_message>
<xml_diff>
--- a/express-routes/portfolio/items/items.xlsx
+++ b/express-routes/portfolio/items/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meatch/MeatchPod/WEBWORKS/Gohman-Docker/html/mitchellgohman.local/express-routes/portfolio/items/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8F1625-D1B4-F846-9FF4-7CBC151F97DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83E4831-5565-1E47-9A58-97EBBEFFFC83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="27220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="109">
-  <si>
-    <t>id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="109">
   <si>
     <t>showHide</t>
   </si>
@@ -301,8 +298,51 @@
     <t>My wife Christin Designed and I developed this Wordpress web application. Custom theme, tailored to client needs.</t>
   </si>
   <si>
+    <t>React/Redux/Context, Laravel, Docker for Local Development, Styled-Components, Less, Accessibility and Training, Custom Theme, HTML, CSS, MYSQL, Decision Trees, Responsive and Mobile First, Shared Libraries, Legacy Zend, Draw.io Diagramming, NPM Library, generating graphic assets (jpgs, pngs, svg).</t>
+  </si>
+  <si>
+    <t>Worked with a Designer to build this Wordpress website that provides Home Listings in LA and Promotes the business.</t>
+  </si>
+  <si>
+    <t>Team CrossFit Academy and I go way back, as I not only Developed and maintained thier website, I also trained with them. Truly an amazing service, and the owner gave me a lot of creative freedom with the website to help promote their business and inform their clientelle.</t>
+  </si>
+  <si>
+    <t>Developed a Customer Relationship Manager for Landmark to assist in keeping track of lead gernation, and reduce overcalling potential customers.</t>
+  </si>
+  <si>
+    <t>Worked wioth designer to create this non-traditional layout. A lot of fun challenges in this project.</t>
+  </si>
+  <si>
+    <t>Designed and developed this website, including the illustrations/graphics, color scheme translated into a Wordpress application to promote the owner, her business, and products.</t>
+  </si>
+  <si>
+    <t>Designed and developed this custom Wordpress theme.</t>
+  </si>
+  <si>
+    <t>A static personal portfolio for Sean Dollins. Sean designed it, and I translated it to web.</t>
+  </si>
+  <si>
+    <t>Custom web applicaton using out of the box php, mysql, javascript, html and css.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;My wife, (&lt;a href='https://christinagohman.com' target='xtina'&gt;Christina Gohman&lt;/a&gt;) desaigned and I developed this Wordpress Custom theme for our Wedding. &lt;/&gt;
+&lt;p&gt;It was used to keep all of our guests informed, and boy did that make all the difference in the world. Still one of my favorite designs, is that cause it was my wedding? Nah.&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t>Converted web application to React/Redux/Context. Also employs front and back servers for security, Authorize.net shopping cart for Catlogue order form, Bidding Application,. Laravel, Laravel Corcel Wordpress, Styled-Components, Less, Custom Theme, HTML, CSS, MYSQL, Mongo, Redis Caching, Responsive and Mobile First, Custom Wordpress CMS Plugin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LMS, Custom Design, Responsive, Mobile First, Laravel 5, HTML, CSS, SASS, JS, JQUERY, Bootstrap, and MYSQL, </t>
+  </si>
+  <si>
+    <t>Wordpress, Custom Theme, HTML, CSS, SASS, JS, JQUERY, PHP &amp;amp; MYSQL.</t>
+  </si>
+  <si>
+    <t>Need to update slideshow on home page? Not showing images.</t>
+  </si>
+  <si>
     <t>&lt;p&gt;
-    Formerly Montrose Travel, Corporate Travel Management (CTM) handles all sorts of travel needs. I  helped to develop and maintain their Loyalty appliedctions which serve Banks and Credit Unions, letting their customers use their points to book a Flight, Hotel, Car, Cruises, and Travel Packages. 
+    Formerly Montrose Travel, Corporate Travel Management (CTM) handles all sorts of travel needs. I  helped to develop and maintain their Loyalty applications which serve Banks and Credit Unions, letting their customers use their points to book a Flight, Hotel, Car, Cruises, and Travel Packages. 
 &lt;/p&gt;
 &lt;p&gt;
     CTM has given me the opportunity to work in large teams (Agile) with many developers, quality assurance (QA), Scrum Masters, Product Managers, Business Analysts, Dev Managers, etc. Working on this team has expanded my ability to not only work with others, but to share code. 
@@ -324,50 +364,10 @@
 &lt;/ul&gt;</t>
   </si>
   <si>
-    <t>React/Redux/Context, Laravel, Docker for Local Development, Styled-Components, Less, Accessibility and Training, Custom Theme, HTML, CSS, MYSQL, Decision Trees, Responsive and Mobile First, Shared Libraries, Legacy Zend, Draw.io Diagramming, NPM Library, generating graphic assets (jpgs, pngs, svg).</t>
-  </si>
-  <si>
-    <t>Worked with a Designer to build this Wordpress website that provides Home Listings in LA and Promotes the business.</t>
-  </si>
-  <si>
-    <t>Team CrossFit Academy and I go way back, as I not only Developed and maintained thier website, I also trained with them. Truly an amazing service, and the owner gave me a lot of creative freedom with the website to help promote their business and inform their clientelle.</t>
-  </si>
-  <si>
-    <t>Developed a Customer Relationship Manager for Landmark to assist in keeping track of lead gernation, and reduce overcalling potential customers.</t>
-  </si>
-  <si>
-    <t>Worked wioth designer to create this non-traditional layout. A lot of fun challenges in this project.</t>
-  </si>
-  <si>
-    <t>Designed and developed this website, including the illustrations/graphics, color scheme translated into a Wordpress application to promote the owner, her business, and products.</t>
-  </si>
-  <si>
-    <t>Designed and developed this custom Wordpress theme.</t>
-  </si>
-  <si>
-    <t>A static personal portfolio for Sean Dollins. Sean designed it, and I translated it to web.</t>
-  </si>
-  <si>
-    <t>Custom web applicaton using out of the box php, mysql, javascript, html and css.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;My wife, (&lt;a href='https://christinagohman.com' target='xtina'&gt;Christina Gohman&lt;/a&gt;) desaigned and I developed this Wordpress Custom theme for our Wedding. &lt;/&gt;
-&lt;p&gt;It was used to keep all of our guests informed, and boy did that make all the difference in the world. Still one of my favorite designs, is that cause it was my wedding? Nah.&lt;/p&gt; </t>
-  </si>
-  <si>
-    <t>Converted web application to React/Redux/Context. Also employs front and back servers for security, Authorize.net shopping cart for Catlogue order form, Bidding Application,. Laravel, Laravel Corcel Wordpress, Styled-Components, Less, Custom Theme, HTML, CSS, MYSQL, Mongo, Redis Caching, Responsive and Mobile First, Custom Wordpress CMS Plugin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LMS, Custom Design, Responsive, Mobile First, Laravel 5, HTML, CSS, SASS, JS, JQUERY, Bootstrap, and MYSQL, </t>
-  </si>
-  <si>
-    <t>Wordpress, Custom Theme, HTML, CSS, SASS, JS, JQUERY, PHP &amp;amp; MYSQL.</t>
-  </si>
-  <si>
-    <t>Need to update slideshow on home page? Not showing images.</t>
-  </si>
-  <si>
-    <t>pdfs</t>
+    <t>padded</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -1224,16 +1224,15 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="1" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="45" style="1" customWidth="1"/>
-    <col min="6" max="7" width="88" style="2" customWidth="1"/>
-    <col min="8" max="8" width="45.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="53.6640625" style="1" customWidth="1"/>
+    <col min="1" max="5" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="45" style="1" customWidth="1"/>
+    <col min="7" max="8" width="88" style="2" customWidth="1"/>
+    <col min="9" max="9" width="45.83203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="58.1640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="69.1640625" style="1" customWidth="1"/>
     <col min="12" max="13" width="7.83203125" style="1" customWidth="1"/>
@@ -1241,688 +1240,748 @@
     <col min="15" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" ht="17">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:14" ht="18" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="1">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="34">
-      <c r="A2" s="1">
-        <v>22</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>22</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:14" ht="18" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="1">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="119">
-      <c r="A3" s="1">
+      <c r="G3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="18" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="1">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="18" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="1">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="G5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="18" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="1">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="18" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="1">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="18" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="1">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="18" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="1">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="18" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="1">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="18" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="1">
         <v>11</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1">
         <v>0</v>
       </c>
-      <c r="D3" s="1">
-        <v>21</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="E11" s="1">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="18" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="18" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="1">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="18" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="1">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>13</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="18" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="1">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>14</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="18" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="1">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="18" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" s="1">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
         <v>16</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="F17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="18" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="1">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
         <v>17</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="F18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="18" customHeight="1">
+      <c r="A19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
         <v>18</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="409.6">
-      <c r="A4" s="1">
-        <v>18</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="F19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="18" customHeight="1">
+      <c r="A20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="1">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="E20" s="1">
         <v>19</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="85">
-      <c r="A5" s="1">
-        <v>17</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="68">
-      <c r="A6" s="1">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>16</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="51">
-      <c r="A7" s="1">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>15</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="34">
-      <c r="A8" s="1">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>14</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="34">
-      <c r="A9" s="1">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="F20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="18" customHeight="1">
+      <c r="A21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="1">
-        <v>13</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="51">
-      <c r="A10" s="1">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <v>12</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="34">
-      <c r="A11" s="1">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="34">
-      <c r="A12" s="1">
+      <c r="C21" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="17">
-      <c r="A13" s="1">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1">
-        <v>9</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="85">
-      <c r="A14" s="1">
-        <v>8</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1">
-        <v>8</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="34">
-      <c r="A15" s="1">
-        <v>5</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1">
-        <v>5</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="17">
-      <c r="A16" s="1">
-        <v>7</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1">
-        <v>7</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="17">
-      <c r="A17" s="1">
-        <v>6</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
-        <v>6</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="17">
-      <c r="A18" s="1">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1">
-        <v>4</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="17">
-      <c r="A19" s="1">
-        <v>3</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1">
-        <v>3</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="17">
-      <c r="A20" s="1">
-        <v>2</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1">
-        <v>2</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="17">
-      <c r="A21" s="1">
-        <v>1</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="1">
+        <v>20</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G21" s="2" t="s">
+      <c r="I21" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="L21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Portfolio: Removed sortOrder column from spreasheets
</commit_message>
<xml_diff>
--- a/express-routes/portfolio/items/items.xlsx
+++ b/express-routes/portfolio/items/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meatch/MeatchPod/WEBWORKS/Gohman-Docker/html/mitchellgohman.local/express-routes/portfolio/items/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83E4831-5565-1E47-9A58-97EBBEFFFC83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED039BF-542F-5A4C-8DB8-BD546A566045}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="27220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="108">
   <si>
     <t>showHide</t>
   </si>
   <si>
     <t>archived</t>
-  </si>
-  <si>
-    <t>sortOrder</t>
   </si>
   <si>
     <t>title</t>
@@ -1220,32 +1217,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="1" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="45" style="1" customWidth="1"/>
-    <col min="7" max="8" width="88" style="2" customWidth="1"/>
-    <col min="9" max="9" width="45.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="58.1640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="69.1640625" style="1" customWidth="1"/>
-    <col min="12" max="13" width="7.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="102.33203125" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="45" style="1" customWidth="1"/>
+    <col min="6" max="7" width="88" style="2" customWidth="1"/>
+    <col min="8" max="8" width="45.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="58.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="69.1640625" style="1" customWidth="1"/>
+    <col min="11" max="12" width="7.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="102.33203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1256,20 +1253,20 @@
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>6</v>
@@ -1280,708 +1277,645 @@
       <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:13" ht="18" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="18" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="1">
-        <v>20</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
       </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="18" customHeight="1">
+    </row>
+    <row r="3" spans="1:13" ht="18" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" s="1">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
       </c>
-      <c r="E3" s="1">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="18" customHeight="1">
+      <c r="L3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="18" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="1">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="1">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="18" customHeight="1">
+    </row>
+    <row r="5" spans="1:13" ht="18" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B5" s="1">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="1">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="18" customHeight="1">
+      <c r="L5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="18" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" s="1">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" s="1">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="18" customHeight="1">
+    </row>
+    <row r="7" spans="1:13" ht="18" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" s="1">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
       </c>
-      <c r="E7" s="1">
-        <v>6</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="18" customHeight="1">
+      <c r="L7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="18" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
       </c>
-      <c r="E8" s="1">
-        <v>7</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="18" customHeight="1">
+      <c r="L8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="18" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="1">
-        <v>8</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>37</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="18" customHeight="1">
+        <v>13</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="18" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="18" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="18" customHeight="1">
-      <c r="A11" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="1">
-        <v>11</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
-      <c r="E11" s="1">
-        <v>10</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="E11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="18" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="1">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="18" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B12" s="1">
-        <v>10</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
-      <c r="E12" s="1">
-        <v>11</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>48</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="18" customHeight="1">
+    </row>
+    <row r="13" spans="1:13" ht="18" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13" s="1">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
       </c>
-      <c r="E13" s="1">
-        <v>12</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="E13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="18" customHeight="1">
+      <c r="L13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="18" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B14" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M14" s="1" t="s">
+    </row>
+    <row r="15" spans="1:13" ht="18" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="18" customHeight="1">
-      <c r="A15" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B15" s="1">
-        <v>7</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
       </c>
-      <c r="E15" s="1">
-        <v>14</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="E15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>66</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="18" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="18" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16" s="1">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="E16" s="1">
-        <v>15</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>59</v>
       </c>
       <c r="K16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="18" customHeight="1">
+    </row>
+    <row r="17" spans="1:12" ht="18" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B17" s="1">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
-      <c r="E17" s="1">
-        <v>16</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="E17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="18" customHeight="1">
+      <c r="L17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="18" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B18" s="1">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="E18" s="1">
-        <v>17</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="E18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>69</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="18" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="18" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B19" s="1">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
       </c>
-      <c r="E19" s="1">
-        <v>18</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="E19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>73</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="18" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="18" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" s="1">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
       </c>
-      <c r="E20" s="1">
-        <v>19</v>
-      </c>
-      <c r="F20" s="1" t="s">
+      <c r="E20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="18" customHeight="1">
+    </row>
+    <row r="21" spans="1:12" ht="18" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B21" s="1">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
       </c>
-      <c r="E21" s="1">
-        <v>20</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="E21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>81</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Portfolio: Fleshing Out Portfolio Profile and Navigation
</commit_message>
<xml_diff>
--- a/express-routes/portfolio/items/items.xlsx
+++ b/express-routes/portfolio/items/items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meatch/MeatchPod/WEBWORKS/Gohmans/christinagohman.local/express-routes/portfolio/items/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4102AD9F-6C10-A244-AD2A-D7382231327B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11944E8-196E-8B47-BC60-882D035A06D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3300" windowWidth="68800" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16120" yWindow="29260" windowWidth="38400" windowHeight="22080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,6 @@
     <t>InDesign, Photoshop, Illustrator</t>
   </si>
   <si>
-    <t>Donny Osmond Home Furniture Catalog / Editorial Design / Hangtag</t>
-  </si>
-  <si>
     <t xml:space="preserve">Editorial Design  </t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t xml:space="preserve">Print + Digital </t>
   </si>
   <si>
-    <t>Scott Living (SL) Furniture Catalog / Editorial Design, Showroom Banners / Hang-tags</t>
-  </si>
-  <si>
     <t>Layout aesthetic + developing working files, complying with the evolving new entity of SL / SBG. Collecting data, adjusting studio photography, page and spread layouts, cover + developing signature data for print.</t>
   </si>
   <si>
@@ -68,9 +62,6 @@
   </si>
   <si>
     <t>POP / Editorial Design / Give-Aways</t>
-  </si>
-  <si>
-    <t>Coaster Furniture Editorial, POP and Give-Aways. *give-away samples available*</t>
   </si>
   <si>
     <t>Illustrator, InDesign, Photoshop</t>
@@ -165,13 +156,22 @@
     <t>development</t>
   </si>
   <si>
-    <t>highlghts</t>
-  </si>
-  <si>
     <t>link</t>
   </si>
   <si>
     <t>pdfs</t>
+  </si>
+  <si>
+    <t>highlights</t>
+  </si>
+  <si>
+    <t>Donny Osmond Home&lt;br /&gt; Furniture Catalog / Editorial Design / Hangtag</t>
+  </si>
+  <si>
+    <t>Scott Living (SL)&lt;br /&gt; Furniture Catalog / Editorial Design, Showroom Banners / Hang-tags</t>
+  </si>
+  <si>
+    <t>Coaster&lt;br /&gt; Furniture Editorial, POP and Give-Aways. *give-away samples available*</t>
   </si>
 </sst>
 </file>
@@ -1040,9 +1040,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="215" zoomScaleNormal="215" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1"/>
@@ -1063,48 +1063,48 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="18" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1113,13 +1113,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>1</v>
@@ -1128,22 +1128,22 @@
         <v>2</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="K2" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="18" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -1152,37 +1152,37 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="18" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -1191,31 +1191,31 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="I4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="K4" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="18" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -1224,30 +1224,30 @@
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="K5" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="18" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -1256,28 +1256,28 @@
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M6" s="4"/>
     </row>

</xml_diff>

<commit_message>
Portfolio: Replaced Gallery Nav Images with full color updated PDFs
</commit_message>
<xml_diff>
--- a/express-routes/portfolio/items/items.xlsx
+++ b/express-routes/portfolio/items/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meatch/MeatchPod/WEBWORKS/Gohmans/christinagohman.local/express-routes/portfolio/items/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11944E8-196E-8B47-BC60-882D035A06D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F4EBE6-FF46-534E-A344-DB12CE8F13C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16120" yWindow="29260" windowWidth="38400" windowHeight="22080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,12 +108,6 @@
     <t>https://perennialstrength.com/</t>
   </si>
   <si>
-    <t>2016.pdf, 2017.pdf, 2018.pdf</t>
-  </si>
-  <si>
-    <t>2017-2018.pdf, 2018-2019.pdf</t>
-  </si>
-  <si>
     <t>1.Donny-Osmond</t>
   </si>
   <si>
@@ -172,6 +166,12 @@
   </si>
   <si>
     <t>Coaster&lt;br /&gt; Furniture Editorial, POP and Give-Aways. *give-away samples available*</t>
+  </si>
+  <si>
+    <t>2016.pdf,2017.pdf,2018.pdf</t>
+  </si>
+  <si>
+    <t>2017-2018.pdf,2018-2019.pdf</t>
   </si>
 </sst>
 </file>
@@ -1040,9 +1040,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="215" zoomScaleNormal="215" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="215" zoomScaleNormal="215" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1"/>
@@ -1063,48 +1063,48 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="18" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1119,7 +1119,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>1</v>
@@ -1134,16 +1134,16 @@
         <v>5</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="18" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -1158,7 +1158,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>9</v>
@@ -1173,16 +1173,16 @@
         <v>11</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="18" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -1197,7 +1197,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>9</v>
@@ -1209,13 +1209,13 @@
         <v>15</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="18" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -1242,12 +1242,12 @@
         <v>20</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="18" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -1274,7 +1274,7 @@
         <v>25</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Portfolio: Updated Items data
</commit_message>
<xml_diff>
--- a/express-routes/portfolio/items/items.xlsx
+++ b/express-routes/portfolio/items/items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meatch/MeatchPod/WEBWORKS/Gohmans/christinagohman.local/express-routes/portfolio/items/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F4EBE6-FF46-534E-A344-DB12CE8F13C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B8A5A6-28D0-EC4F-96E7-1F5491D1DDD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16120" yWindow="29260" windowWidth="38400" windowHeight="22080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17980" yWindow="29260" windowWidth="33600" windowHeight="19080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>title</t>
   </si>
@@ -58,21 +58,12 @@
     <t>Scott Brothers Global 2019 Tennessee Summit Attendee. Joined with other licensees for the introduction and reveal of the Scott Living brand. </t>
   </si>
   <si>
-    <t>COASTER FURNITURE</t>
-  </si>
-  <si>
     <t>POP / Editorial Design / Give-Aways</t>
   </si>
   <si>
     <t>Illustrator, InDesign, Photoshop</t>
   </si>
   <si>
-    <t xml:space="preserve">TOP: create a fun and engaging visual informational campaign that included a brochure, stand, poster, and email blast for PROP 65. Explored visual engagement to take the viewer on a tour of the complex topic.
-BOTTOM: Worked with freelance artist to create and manipulate characters. Developed an array of patterns in Illustrator to be displayed on “giveaways” such as recycled bags, umbrellas and other media.
-Created mocks and hangtag. 
-Samples available.  </t>
-  </si>
-  <si>
     <t>Web Collateral</t>
   </si>
   <si>
@@ -85,11 +76,6 @@
     <t>InDesign, Photoshop, Illustrator, Mailchimp, Dreamweaver, ISSUU</t>
   </si>
   <si>
-    <t>TOP: communicate with the audience about an error from the original email. The goal was to present something fun and convey accurate information to the end user minimizing frustration and acknowledging the mistake. 
-2: Web slides hosted on one of the Coaster Company websites. Based on the time of year, slides were created to tell a story of a particular event: market show announcements, social media links, special promotions. 
-3: Develop a visual web portal that allows end user to access web friendly converted print material: catalogs, images and informational spread sheets.</t>
-  </si>
-  <si>
     <t>PERENNIAL STRENGTH</t>
   </si>
   <si>
@@ -172,6 +158,25 @@
   </si>
   <si>
     <t>2017-2018.pdf,2018-2019.pdf</t>
+  </si>
+  <si>
+    <t>CF PRINT MEDIA</t>
+  </si>
+  <si>
+    <t>CF WEB MEDIA</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;TOP: create a fun and engaging visual informational campaign that included a brochure, stand, poster, and email blast for PROP 65. Explored visual engagement to take the viewer on a tour of the complex topic.&lt;/p&gt;
+&lt;p&gt;BOTTOM: Worked with freelance artist to create and manipulate characters. Developed an array of patterns in Illustrator to be displayed on “giveaways” such as recycled bags, umbrellas and other media.&lt;/p&gt;
+&lt;p&gt;
+    Created mocks and hangtag. 
+    Samples available. &lt;br/&gt;
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;TOP: communicate with the audience about an error from the original email. The goal was to present something fun and convey accurate information to the end user minimizing frustration and acknowledging the mistake. &lt;/p&gt;
+&lt;p&gt;2: Web slides hosted on one of the Coaster Company websites. Based on the time of year, slides were created to tell a story of a particular event: market show announcements, social media links, special promotions. &lt;/p&gt;
+&lt;p&gt;3: Develop a visual web portal that allows end user to access web friendly converted print material: catalogs, images and informational spread sheets.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -1040,9 +1045,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="215" zoomScaleNormal="215" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1"/>
@@ -1063,48 +1068,48 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="18" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1119,7 +1124,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>1</v>
@@ -1134,16 +1139,16 @@
         <v>5</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="18" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -1158,7 +1163,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>9</v>
@@ -1173,16 +1178,16 @@
         <v>11</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="18" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -1191,31 +1196,31 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="18" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -1224,30 +1229,30 @@
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="I5" s="5" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="18" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -1256,28 +1261,28 @@
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M6" s="4"/>
     </row>

</xml_diff>

<commit_message>
Updated portfolio with Full Petential
</commit_message>
<xml_diff>
--- a/express-routes/portfolio/items/items.xlsx
+++ b/express-routes/portfolio/items/items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meatch/MeatchPod/WEBWORKS/Gohmans/christinagohman.local/express-routes/portfolio/items/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FFE96C-6166-E549-B866-66684819762B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AB30B1-16B2-5944-9FAE-03C3C7FA12C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="13900" windowWidth="68800" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="14640" windowWidth="68800" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
   <si>
     <t>title</t>
   </si>
@@ -179,12 +179,31 @@
   <si>
     <t>Donny Osmond himself expressed his gratitude to me personally for the vision created that represents his brand at the 2018 Las Vegas Market Show!</t>
   </si>
+  <si>
+    <t>FULL PETENTIAL</t>
+  </si>
+  <si>
+    <t>Identity, Packaging</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Objective: An internship turned into a paid gig! Created company identity. Assets included illustrative logo, type logo, color platform, mailers, and packaging of canine and feline treats.&lt;/p&gt;
+&lt;p&gt;Packaged samples available.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>6.Full-Petential</t>
+  </si>
+  <si>
+    <t>Full Petential Identity</t>
+  </si>
+  <si>
+    <t>Print, Packaging</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1044,19 +1063,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="10.83203125" style="3"/>
     <col min="4" max="4" width="25.83203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="45.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="45.1640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="76.33203125" style="5" customWidth="1"/>
     <col min="7" max="7" width="29.33203125" style="5" customWidth="1"/>
     <col min="8" max="8" width="45.1640625" style="5" customWidth="1"/>
     <col min="9" max="9" width="59.6640625" style="5" customWidth="1"/>
@@ -1067,7 +1086,7 @@
     <col min="14" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="18" customHeight="1">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -1108,7 +1127,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="18" customHeight="1">
+    <row r="2" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -1147,7 +1166,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="18" customHeight="1">
+    <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
@@ -1186,7 +1205,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="18" customHeight="1">
+    <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -1219,7 +1238,7 @@
       </c>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:13" ht="18" customHeight="1">
+    <row r="5" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -1251,7 +1270,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="18" customHeight="1">
+    <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1286,6 +1305,38 @@
         <v>18</v>
       </c>
       <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="3">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>